<commit_message>
Populate script fixed period issue, old upload files removed
</commit_message>
<xml_diff>
--- a/public/upload/annuals/11.2015.xlsx
+++ b/public/upload/annuals/11.2015.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr updateLinks="never" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="390" windowWidth="14940" windowHeight="7275" tabRatio="954" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="390" windowWidth="14940" windowHeight="7275" tabRatio="954" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="ფორმა N1" sheetId="42" r:id="rId1"/>
@@ -79,7 +79,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="2">'ფორმა N3'!$A$1:$E$42</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="3">'ფორმა N4'!$A$1:$E$89</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="4">'ფორმა N4.1'!$A$1:$E$38</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="8">'ფორმა N5'!$A$1:$D$86</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="8">'ფორმა N5'!$A$1:$D$92</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="14">'ფორმა N6'!$A$1:$D$32</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="16">'ფორმა N7'!$A$1:$E$90</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="19">'ფორმა N9'!$A$1:$K$52</definedName>
@@ -87,12 +87,12 @@
     <definedName name="_xlnm.Print_Area" localSheetId="21">'ფორმა N9.2'!$A$1:$J$36</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="27">'ფორმა N9.7.1'!$A$1:$N$42</definedName>
   </definedNames>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1299" uniqueCount="616">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1304" uniqueCount="616">
   <si>
     <t>პრემია</t>
   </si>
@@ -1870,12 +1870,6 @@
     </r>
   </si>
   <si>
-    <t>გარე რეკლამის ხარჯი *</t>
-  </si>
-  <si>
-    <t>1.2.8.6</t>
-  </si>
-  <si>
     <t>* ბილბორდი, ლაით ბოქსი, ქუჩაში დამონტაჟებული ეკრანი, სატრანსპორტო საშუალებებზე განთავსებული რეკლამა და სხვა.</t>
   </si>
   <si>
@@ -2216,12 +2210,18 @@
   </si>
   <si>
     <t xml:space="preserve">უსასყიდლო                          </t>
+  </si>
+  <si>
+    <t>სსიპ "საარჩევნო სისტემების განვითარების, რეფორმებისა და სწავლების ცენტრიდან" მიღებული სახსრებით გაწეული ხარჯები</t>
+  </si>
+  <si>
+    <t>რეგიონალური პროექტების დაფინანსების ხარჯები</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="5">
     <numFmt numFmtId="164" formatCode="00,000.00"/>
     <numFmt numFmtId="165" formatCode="0,000.00"/>
@@ -2229,7 +2229,7 @@
     <numFmt numFmtId="167" formatCode="dd/mm/yy;@"/>
     <numFmt numFmtId="168" formatCode="\ს\ა\ტ\ე\ლ\ე\ვ\ი\ზ\ი\ო\ \რ\ე\კ\ლ\ა\მ\ა"/>
   </numFmts>
-  <fonts count="39">
+  <fonts count="41">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -2478,8 +2478,17 @@
       <family val="1"/>
       <charset val="204"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Merriweather"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Merriweather"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2516,8 +2525,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD9EAD3"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="44">
+  <borders count="48">
     <border>
       <left/>
       <right/>
@@ -3068,6 +3083,58 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -3082,7 +3149,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="473">
+  <cellXfs count="478">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
@@ -4553,8 +4620,22 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="39" fillId="7" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="7" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="7" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="7" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="11">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2"/>
     <cellStyle name="Normal 3" xfId="3"/>
     <cellStyle name="Normal 4" xfId="4"/>
@@ -4565,7 +4646,6 @@
     <cellStyle name="Normal 5 3" xfId="9"/>
     <cellStyle name="Normal 5 3 2" xfId="10"/>
     <cellStyle name="Normal_FORMEBI" xfId="1"/>
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -7954,13 +8034,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>775607</xdr:colOff>
-      <xdr:row>81</xdr:row>
+      <xdr:row>87</xdr:row>
       <xdr:rowOff>171450</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>1318532</xdr:colOff>
-      <xdr:row>81</xdr:row>
+      <xdr:row>87</xdr:row>
       <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -7998,13 +8078,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>2086495</xdr:colOff>
-      <xdr:row>81</xdr:row>
+      <xdr:row>87</xdr:row>
       <xdr:rowOff>180975</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>4827200</xdr:colOff>
-      <xdr:row>81</xdr:row>
+      <xdr:row>87</xdr:row>
       <xdr:rowOff>182563</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -8135,7 +8215,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="ფორმა N1"/>
@@ -8220,7 +8300,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="ფორმა N1"/>
@@ -8301,7 +8381,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink3.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="ფორმა N1"/>
@@ -8344,9 +8424,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Стандартная">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -8384,7 +8464,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Стандартная">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -8418,6 +8498,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -8452,9 +8533,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Стандартная">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -8627,7 +8709,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -8713,7 +8795,7 @@
       <c r="J4" s="367"/>
       <c r="K4" s="367"/>
       <c r="L4" s="379" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
     </row>
     <row r="5" spans="1:12" s="312" customFormat="1">
@@ -8740,7 +8822,7 @@
         <v>276</v>
       </c>
       <c r="E6" s="373" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
       <c r="F6" s="368"/>
       <c r="G6" s="367"/>
@@ -9473,7 +9555,7 @@
     <dataValidation type="textLength" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="პირადი ნომრის შევსების წესი" error="პირადი ნომერი უნდა შეიცავდეს 11 სიმბოლოს" sqref="F12:H31">
       <formula1>11</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="შემოსავლის ტიპის შევსების წესი" error="ველში იწერება შემდეგი შემოსავლის ტიპებიდან ერთ-ერთი:&#10;- ფულადი შემოწირულობები&#10;- არაფულადი შემოწირულობები&#10;- საწევრო&#10;" sqref="C12:C31">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="შემოსავლის ტიპის შევსების წესი" error="ველში იწერება შემდეგი შემოსავლის ტიპებიდან ერთ-ერთი:_x000a_- ფულადი შემოწირულობები_x000a_- არაფულადი შემოწირულობები_x000a_- საწევრო_x000a_" sqref="C12:C31">
       <formula1>"ფულადი შემოწირულობა, არაფულადი შემოწირულობა, საწევრო"</formula1>
     </dataValidation>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" error="თვე/დღე/წელი" prompt="თვე/დღე/წელი" sqref="B12:B31"/>
@@ -9485,7 +9567,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I39"/>
   <sheetViews>
     <sheetView showGridLines="0" view="pageBreakPreview" zoomScale="70" zoomScaleSheetLayoutView="70" workbookViewId="0">
@@ -9519,7 +9601,7 @@
       </c>
       <c r="B2" s="77"/>
       <c r="C2" s="454" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="D2" s="454"/>
       <c r="E2" s="91"/>
@@ -9553,7 +9635,7 @@
     <row r="6" spans="1:5">
       <c r="A6" s="80"/>
       <c r="B6" s="80" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
       <c r="C6" s="81"/>
       <c r="D6" s="81"/>
@@ -9830,7 +9912,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -9883,7 +9965,7 @@
       <c r="G2" s="299"/>
       <c r="H2" s="299"/>
       <c r="I2" s="454" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="J2" s="454"/>
     </row>
@@ -9915,7 +9997,7 @@
       <c r="A5" s="80"/>
       <c r="B5" s="80"/>
       <c r="C5" s="80" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
       <c r="D5" s="80"/>
       <c r="E5" s="80"/>
@@ -10481,7 +10563,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -10527,7 +10609,7 @@
       <c r="E2" s="77"/>
       <c r="F2" s="77"/>
       <c r="G2" s="454" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="H2" s="454"/>
     </row>
@@ -10556,7 +10638,7 @@
     <row r="5" spans="1:8" ht="15">
       <c r="A5" s="80"/>
       <c r="B5" s="80" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="C5" s="80"/>
       <c r="D5" s="80"/>
@@ -11020,7 +11102,7 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -11069,7 +11151,7 @@
       <c r="E2" s="77"/>
       <c r="F2" s="77"/>
       <c r="G2" s="454" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="H2" s="454"/>
     </row>
@@ -11100,7 +11182,7 @@
       <c r="B5" s="80"/>
       <c r="C5" s="80"/>
       <c r="D5" s="80" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
       <c r="E5" s="80"/>
       <c r="F5" s="80"/>
@@ -11580,7 +11662,7 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -11639,7 +11721,7 @@
       <c r="I3" s="77"/>
       <c r="J3" s="299"/>
       <c r="K3" s="454" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="L3" s="454"/>
     </row>
@@ -11677,7 +11759,7 @@
       <c r="A6" s="80"/>
       <c r="B6" s="80"/>
       <c r="C6" s="80" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
       <c r="D6" s="80"/>
       <c r="E6" s="80"/>
@@ -12379,7 +12461,7 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:I32"/>
   <sheetViews>
@@ -12412,7 +12494,7 @@
       </c>
       <c r="B2" s="76"/>
       <c r="C2" s="454" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="D2" s="455"/>
     </row>
@@ -12446,7 +12528,7 @@
         <v>#REF!</v>
       </c>
       <c r="B6" s="122" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="C6" s="122"/>
       <c r="D6" s="58"/>
@@ -12714,7 +12796,7 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I89"/>
   <sheetViews>
     <sheetView showGridLines="0" view="pageBreakPreview" zoomScale="70" zoomScaleSheetLayoutView="70" workbookViewId="0">
@@ -12751,7 +12833,7 @@
       </c>
       <c r="B2" s="77"/>
       <c r="C2" s="454" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="D2" s="454"/>
       <c r="E2" s="469"/>
@@ -12797,7 +12879,7 @@
     <row r="6" spans="1:8" ht="15.75" customHeight="1">
       <c r="A6" s="80"/>
       <c r="B6" s="80" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
       <c r="C6" s="81"/>
       <c r="D6" s="81"/>
@@ -13666,7 +13748,7 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:K93"/>
   <sheetViews>
@@ -13701,7 +13783,7 @@
       <c r="B2" s="123"/>
       <c r="C2" s="77"/>
       <c r="D2" s="230" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="E2" s="105"/>
     </row>
@@ -13728,7 +13810,7 @@
         <v>#REF!</v>
       </c>
       <c r="B5" s="122" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
       <c r="C5" s="122"/>
       <c r="D5" s="58"/>
@@ -13879,7 +13961,7 @@
         <v>1215</v>
       </c>
       <c r="B18" s="55" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="C18" s="8">
         <v>28891</v>
@@ -14635,7 +14717,7 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:K25"/>
   <sheetViews>
@@ -14687,7 +14769,7 @@
       <c r="G2" s="76"/>
       <c r="H2" s="76"/>
       <c r="I2" s="454" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="J2" s="455"/>
       <c r="K2" s="105"/>
@@ -14712,7 +14794,7 @@
       </c>
       <c r="B4" s="76"/>
       <c r="C4" s="76" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
       <c r="D4" s="76"/>
       <c r="E4" s="76"/>
@@ -14836,10 +14918,10 @@
         <v>1</v>
       </c>
       <c r="B10" s="436" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
       <c r="C10" s="437" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="D10" s="438" t="s">
         <v>221</v>
@@ -14865,10 +14947,10 @@
         <v>2</v>
       </c>
       <c r="B11" s="441" t="s">
+        <v>580</v>
+      </c>
+      <c r="C11" s="443" t="s">
         <v>582</v>
-      </c>
-      <c r="C11" s="443" t="s">
-        <v>584</v>
       </c>
       <c r="D11" s="441" t="s">
         <v>221</v>
@@ -15043,7 +15125,7 @@
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -15090,7 +15172,7 @@
       <c r="E2" s="76"/>
       <c r="F2" s="76"/>
       <c r="G2" s="169" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="H2" s="168"/>
     </row>
@@ -15121,7 +15203,7 @@
       <c r="A5" s="227"/>
       <c r="B5" s="227"/>
       <c r="C5" s="227" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="D5" s="227"/>
       <c r="E5" s="227"/>
@@ -15202,7 +15284,7 @@
         <v>221</v>
       </c>
       <c r="F10" s="178" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
       <c r="G10" s="179">
         <f>IF(ISBLANK(B10),"",G9+C10-D10)</f>
@@ -15225,7 +15307,7 @@
         <v>221</v>
       </c>
       <c r="F11" s="178" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
       <c r="G11" s="179">
         <f t="shared" ref="G11:G38" si="0">IF(ISBLANK(B11),"",G10+C11-D11)</f>
@@ -15248,7 +15330,7 @@
         <v>221</v>
       </c>
       <c r="F12" s="178" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
       <c r="G12" s="179">
         <f t="shared" si="0"/>
@@ -15271,7 +15353,7 @@
         <v>221</v>
       </c>
       <c r="F13" s="178" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="G13" s="179">
         <f t="shared" si="0"/>
@@ -15294,7 +15376,7 @@
         <v>221</v>
       </c>
       <c r="F14" s="178" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
       <c r="G14" s="179">
         <f t="shared" si="0"/>
@@ -15317,7 +15399,7 @@
         <v>221</v>
       </c>
       <c r="F15" s="178" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="G15" s="179">
         <f t="shared" si="0"/>
@@ -15340,7 +15422,7 @@
         <v>221</v>
       </c>
       <c r="F16" s="178" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
       <c r="G16" s="179">
         <f t="shared" si="0"/>
@@ -15363,7 +15445,7 @@
         <v>221</v>
       </c>
       <c r="F17" s="178" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
       <c r="G17" s="179">
         <f t="shared" si="0"/>
@@ -15386,7 +15468,7 @@
         <v>221</v>
       </c>
       <c r="F18" s="178" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
       <c r="G18" s="179">
         <f t="shared" si="0"/>
@@ -15409,7 +15491,7 @@
         <v>221</v>
       </c>
       <c r="F19" s="178" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
       <c r="G19" s="179">
         <f t="shared" si="0"/>
@@ -15432,7 +15514,7 @@
         <v>221</v>
       </c>
       <c r="F20" s="178" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
       <c r="G20" s="179">
         <f t="shared" si="0"/>
@@ -15455,7 +15537,7 @@
         <v>221</v>
       </c>
       <c r="F21" s="178" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
       <c r="G21" s="179">
         <f t="shared" si="0"/>
@@ -15478,7 +15560,7 @@
         <v>221</v>
       </c>
       <c r="F22" s="178" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
       <c r="G22" s="179">
         <f t="shared" si="0"/>
@@ -15501,7 +15583,7 @@
         <v>221</v>
       </c>
       <c r="F23" s="178" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
       <c r="G23" s="179">
         <f t="shared" si="0"/>
@@ -15524,7 +15606,7 @@
         <v>221</v>
       </c>
       <c r="F24" s="178" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
       <c r="G24" s="179">
         <f t="shared" si="0"/>
@@ -15547,7 +15629,7 @@
         <v>221</v>
       </c>
       <c r="F25" s="178" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
       <c r="G25" s="179">
         <f t="shared" si="0"/>
@@ -15570,7 +15652,7 @@
         <v>221</v>
       </c>
       <c r="F26" s="178" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
       <c r="G26" s="179">
         <f t="shared" si="0"/>
@@ -15593,7 +15675,7 @@
         <v>221</v>
       </c>
       <c r="F27" s="178" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
       <c r="G27" s="179">
         <f t="shared" si="0"/>
@@ -15616,7 +15698,7 @@
         <v>221</v>
       </c>
       <c r="F28" s="178" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
       <c r="G28" s="179">
         <f t="shared" si="0"/>
@@ -15639,7 +15721,7 @@
         <v>221</v>
       </c>
       <c r="F29" s="178" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
       <c r="G29" s="179">
         <f t="shared" si="0"/>
@@ -15662,7 +15744,7 @@
         <v>221</v>
       </c>
       <c r="F30" s="181" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
       <c r="G30" s="179">
         <f t="shared" si="0"/>
@@ -15685,7 +15767,7 @@
         <v>221</v>
       </c>
       <c r="F31" s="181" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
       <c r="G31" s="179">
         <f t="shared" si="0"/>
@@ -15708,7 +15790,7 @@
         <v>221</v>
       </c>
       <c r="F32" s="181" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
       <c r="G32" s="179">
         <f t="shared" si="0"/>
@@ -15731,7 +15813,7 @@
         <v>221</v>
       </c>
       <c r="F33" s="181" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
       <c r="G33" s="179">
         <f t="shared" si="0"/>
@@ -15754,7 +15836,7 @@
         <v>221</v>
       </c>
       <c r="F34" s="181" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
       <c r="G34" s="179">
         <f t="shared" si="0"/>
@@ -15777,7 +15859,7 @@
         <v>221</v>
       </c>
       <c r="F35" s="181" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
       <c r="G35" s="179">
         <f t="shared" si="0"/>
@@ -15800,7 +15882,7 @@
         <v>221</v>
       </c>
       <c r="F36" s="181" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="G36" s="179">
         <f t="shared" si="0"/>
@@ -15933,11 +16015,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:I41"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScale="70" zoomScaleSheetLayoutView="70" workbookViewId="0">
+    <sheetView showGridLines="0" view="pageBreakPreview" topLeftCell="A8" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
@@ -15970,7 +16052,7 @@
       </c>
       <c r="B2" s="76"/>
       <c r="C2" s="454" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="D2" s="455"/>
       <c r="E2" s="108"/>
@@ -15997,7 +16079,7 @@
         <v>#REF!</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="C5" s="12"/>
       <c r="E5" s="108"/>
@@ -16420,7 +16502,7 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet8">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -16474,7 +16556,7 @@
       <c r="G2" s="142"/>
       <c r="H2" s="142"/>
       <c r="I2" s="454" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="J2" s="455"/>
       <c r="K2" s="146"/>
@@ -16515,7 +16597,7 @@
         <v>#REF!</v>
       </c>
       <c r="B5" s="122" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
       <c r="C5" s="122"/>
       <c r="D5" s="122"/>
@@ -17453,7 +17535,7 @@
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet12"/>
   <dimension ref="A1:L35"/>
   <sheetViews>
@@ -17507,7 +17589,7 @@
       <c r="F2" s="140"/>
       <c r="G2" s="148"/>
       <c r="H2" s="419" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="I2" s="148"/>
       <c r="J2" s="66"/>
@@ -17553,7 +17635,7 @@
       <c r="B5" s="122"/>
       <c r="C5" s="122"/>
       <c r="D5" s="122" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
       <c r="E5" s="150"/>
       <c r="F5" s="151"/>
@@ -17973,7 +18055,7 @@
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="შევსების წესი" error="შენობა-ნაგებობების ტიპები აირჩიეთ შემდეგი ჩამონათვალიდან:&#10;&#10;- საცხოვრებელი შენობები&#10;- არასაცხოვრებელი შენობები&#10;- სხვა ნაგებობები&#10;- დაუმთავრებელი მშენებლობა" sqref="B9:B27">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="შევსების წესი" error="შენობა-ნაგებობების ტიპები აირჩიეთ შემდეგი ჩამონათვალიდან:_x000a__x000a_- საცხოვრებელი შენობები_x000a_- არასაცხოვრებელი შენობები_x000a_- სხვა ნაგებობები_x000a_- დაუმთავრებელი მშენებლობა" sqref="B9:B27">
       <formula1>"საცხოვრებალი შენობები, არასაცხოვრებელი შენობები, სხვა ნაგებობები, დაუმთავრებელი მშენებლობა"</formula1>
     </dataValidation>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="თვე/დღე/წელი" sqref="G9:G27"/>
@@ -17987,7 +18069,7 @@
 </file>
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet13"/>
   <dimension ref="A1:L54"/>
   <sheetViews>
@@ -18036,7 +18118,7 @@
       <c r="G2" s="140"/>
       <c r="H2" s="146"/>
       <c r="I2" s="419" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="J2" s="153"/>
     </row>
@@ -18077,7 +18159,7 @@
       <c r="C5" s="122"/>
       <c r="D5" s="122"/>
       <c r="E5" s="150" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
       <c r="F5" s="151"/>
       <c r="G5" s="151"/>
@@ -18539,7 +18621,7 @@
 </file>
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -18586,7 +18668,7 @@
       <c r="E2" s="199"/>
       <c r="F2" s="199"/>
       <c r="G2" s="200" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="H2" s="202"/>
     </row>
@@ -18616,7 +18698,7 @@
       <c r="A5" s="204"/>
       <c r="B5" s="204"/>
       <c r="C5" s="204" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
       <c r="D5" s="204"/>
       <c r="E5" s="204"/>
@@ -18870,7 +18952,7 @@
 </file>
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -18925,7 +19007,7 @@
       <c r="I2" s="140"/>
       <c r="J2" s="140"/>
       <c r="K2" s="419" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="15">
@@ -18965,7 +19047,7 @@
       <c r="B5" s="80"/>
       <c r="C5" s="80"/>
       <c r="D5" s="80" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
       <c r="E5" s="228"/>
       <c r="F5" s="229"/>
@@ -19063,28 +19145,28 @@
         <v>1</v>
       </c>
       <c r="B9" s="25" t="s">
+        <v>610</v>
+      </c>
+      <c r="C9" s="25" t="s">
+        <v>599</v>
+      </c>
+      <c r="D9" s="25" t="s">
+        <v>611</v>
+      </c>
+      <c r="E9" s="25" t="s">
         <v>612</v>
       </c>
-      <c r="C9" s="25" t="s">
-        <v>601</v>
-      </c>
-      <c r="D9" s="25" t="s">
+      <c r="F9" s="25" t="s">
         <v>613</v>
-      </c>
-      <c r="E9" s="25" t="s">
-        <v>614</v>
-      </c>
-      <c r="F9" s="25" t="s">
-        <v>615</v>
       </c>
       <c r="G9" s="25">
         <v>1010011415</v>
       </c>
       <c r="H9" s="225" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="I9" s="225" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="J9" s="225"/>
       <c r="K9" s="25"/>
@@ -19094,28 +19176,28 @@
         <v>2</v>
       </c>
       <c r="B10" s="25" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="C10" s="25" t="s">
+        <v>599</v>
+      </c>
+      <c r="D10" s="25" t="s">
+        <v>600</v>
+      </c>
+      <c r="E10" s="25" t="s">
         <v>601</v>
       </c>
-      <c r="D10" s="25" t="s">
+      <c r="F10" s="25" t="s">
         <v>602</v>
-      </c>
-      <c r="E10" s="25" t="s">
-        <v>603</v>
-      </c>
-      <c r="F10" s="25" t="s">
-        <v>604</v>
       </c>
       <c r="G10" s="25">
         <v>53001004062</v>
       </c>
       <c r="H10" s="225" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
       <c r="I10" s="225" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="J10" s="225"/>
       <c r="K10" s="25"/>
@@ -19471,7 +19553,7 @@
 </file>
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -19531,7 +19613,7 @@
       <c r="J2" s="140"/>
       <c r="K2" s="146"/>
       <c r="L2" s="419" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
     </row>
     <row r="3" spans="1:13" customFormat="1" ht="15">
@@ -19574,7 +19656,7 @@
       <c r="B5" s="227"/>
       <c r="C5" s="80"/>
       <c r="D5" s="80" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
       <c r="E5" s="80"/>
       <c r="F5" s="228"/>
@@ -20077,7 +20159,7 @@
 </file>
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -20127,7 +20209,7 @@
       <c r="G2" s="140"/>
       <c r="H2" s="146"/>
       <c r="I2" s="419" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
     </row>
     <row r="3" spans="1:13" customFormat="1" ht="15">
@@ -20164,7 +20246,7 @@
       <c r="B5" s="80"/>
       <c r="C5" s="80"/>
       <c r="D5" s="229" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
       <c r="E5" s="229"/>
       <c r="F5" s="229"/>
@@ -20573,7 +20655,7 @@
 </file>
 
 <file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -20626,7 +20708,7 @@
       <c r="G2" s="76"/>
       <c r="H2" s="76"/>
       <c r="I2" s="169" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="J2" s="168"/>
     </row>
@@ -20661,7 +20743,7 @@
       <c r="A5" s="227"/>
       <c r="B5" s="227"/>
       <c r="C5" s="227" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="D5" s="227"/>
       <c r="E5" s="227"/>
@@ -21227,7 +21309,7 @@
 </file>
 
 <file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N43"/>
   <sheetViews>
     <sheetView showGridLines="0" view="pageBreakPreview" zoomScale="70" zoomScaleSheetLayoutView="70" workbookViewId="0">
@@ -21288,7 +21370,7 @@
       <c r="K2" s="198"/>
       <c r="L2" s="198"/>
       <c r="M2" s="200" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="N2" s="202"/>
     </row>
@@ -21332,7 +21414,7 @@
       <c r="C5" s="204"/>
       <c r="D5" s="204"/>
       <c r="E5" s="205" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
       <c r="F5" s="205"/>
       <c r="G5" s="205"/>
@@ -22041,7 +22123,7 @@
 </file>
 
 <file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet10"/>
   <dimension ref="A1:G733"/>
   <sheetViews>
@@ -25814,7 +25896,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:L42"/>
   <sheetViews>
@@ -25878,7 +25960,7 @@
         <v>#REF!</v>
       </c>
       <c r="B5" s="263" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="C5" s="58"/>
       <c r="D5" s="58"/>
@@ -26288,7 +26370,7 @@
 </file>
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -26300,7 +26382,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I88"/>
   <sheetViews>
     <sheetView showGridLines="0" view="pageBreakPreview" topLeftCell="A28" zoomScale="70" zoomScaleSheetLayoutView="70" workbookViewId="0">
@@ -26334,7 +26416,7 @@
       </c>
       <c r="B2" s="246"/>
       <c r="C2" s="454" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="D2" s="455"/>
       <c r="E2" s="91"/>
@@ -26380,7 +26462,7 @@
         <v/>
       </c>
       <c r="B7" s="80" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="C7" s="81"/>
       <c r="D7" s="81"/>
@@ -26675,7 +26757,7 @@
         <v>289</v>
       </c>
       <c r="B29" s="256" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="C29" s="422">
         <v>480</v>
@@ -27352,7 +27434,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I108"/>
   <sheetViews>
     <sheetView showGridLines="0" view="pageBreakPreview" zoomScale="70" zoomScaleSheetLayoutView="70" workbookViewId="0">
@@ -27385,7 +27467,7 @@
       </c>
       <c r="B2" s="77"/>
       <c r="C2" s="454" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
       <c r="D2" s="454"/>
       <c r="E2" s="91"/>
@@ -27419,7 +27501,7 @@
     <row r="6" spans="1:5">
       <c r="A6" s="80"/>
       <c r="B6" s="80" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="C6" s="81"/>
       <c r="D6" s="81"/>
@@ -28218,7 +28300,7 @@
     <row r="105" spans="1:4">
       <c r="A105" s="188"/>
       <c r="B105" s="188" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="C105" s="188"/>
       <c r="D105" s="195"/>
@@ -28258,7 +28340,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -28311,7 +28393,7 @@
       <c r="G2" s="233"/>
       <c r="H2" s="233"/>
       <c r="I2" s="454" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="J2" s="454"/>
     </row>
@@ -28344,7 +28426,7 @@
       <c r="A5" s="80"/>
       <c r="B5" s="80"/>
       <c r="C5" s="80" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
       <c r="D5" s="80"/>
       <c r="E5" s="80"/>
@@ -28412,10 +28494,10 @@
         <v>1</v>
       </c>
       <c r="B9" s="406" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="C9" s="403" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="D9" s="400">
         <v>1010011415</v>
@@ -28442,10 +28524,10 @@
         <v>2</v>
       </c>
       <c r="B10" s="406" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="C10" s="403" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="D10" s="400">
         <v>1026008465</v>
@@ -28469,10 +28551,10 @@
         <v>3</v>
       </c>
       <c r="B11" s="406" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="C11" s="403" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="D11" s="400">
         <v>58001000338</v>
@@ -28496,10 +28578,10 @@
         <v>4</v>
       </c>
       <c r="B12" s="406" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="C12" s="403" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="D12" s="400">
         <v>1022001763</v>
@@ -28523,10 +28605,10 @@
         <v>5</v>
       </c>
       <c r="B13" s="406" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="C13" s="403" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="D13" s="400">
         <v>1024036647</v>
@@ -28550,10 +28632,10 @@
         <v>6</v>
       </c>
       <c r="B14" s="406" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="C14" s="403" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="D14" s="400">
         <v>46001002506</v>
@@ -28577,10 +28659,10 @@
         <v>7</v>
       </c>
       <c r="B15" s="406" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="C15" s="403" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="D15" s="400">
         <v>1006011079</v>
@@ -28604,10 +28686,10 @@
         <v>8</v>
       </c>
       <c r="B16" s="406" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="C16" s="403" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="D16" s="400">
         <v>1014003443</v>
@@ -28631,10 +28713,10 @@
         <v>9</v>
       </c>
       <c r="B17" s="406" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="C17" s="403" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="D17" s="400">
         <v>1005034665</v>
@@ -28658,10 +28740,10 @@
         <v>10</v>
       </c>
       <c r="B18" s="406" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="C18" s="403" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="D18" s="400">
         <v>1030024961</v>
@@ -28685,10 +28767,10 @@
         <v>11</v>
       </c>
       <c r="B19" s="406" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="C19" s="403" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="D19" s="400">
         <v>1006015862</v>
@@ -28712,10 +28794,10 @@
         <v>12</v>
       </c>
       <c r="B20" s="406" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="C20" s="403" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="D20" s="400">
         <v>12001069159</v>
@@ -28739,10 +28821,10 @@
         <v>13</v>
       </c>
       <c r="B21" s="406" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="C21" s="403" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="D21" s="400">
         <v>1008019822</v>
@@ -28766,10 +28848,10 @@
         <v>14</v>
       </c>
       <c r="B22" s="406" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="C22" s="403" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="D22" s="400">
         <v>1006008165</v>
@@ -28793,10 +28875,10 @@
         <v>15</v>
       </c>
       <c r="B23" s="406" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="C23" s="403" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="D23" s="400">
         <v>12001050813</v>
@@ -28820,10 +28902,10 @@
         <v>16</v>
       </c>
       <c r="B24" s="406" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="C24" s="403" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="D24" s="400">
         <v>14001003911</v>
@@ -28847,10 +28929,10 @@
         <v>17</v>
       </c>
       <c r="B25" s="406" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="C25" s="403" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="D25" s="400">
         <v>1027019748</v>
@@ -28874,10 +28956,10 @@
         <v>18</v>
       </c>
       <c r="B26" s="406" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="C26" s="403" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="D26" s="400">
         <v>16001014254</v>
@@ -28901,10 +28983,10 @@
         <v>19</v>
       </c>
       <c r="B27" s="406" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="C27" s="403" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="D27" s="400">
         <v>1019003796</v>
@@ -28928,10 +29010,10 @@
         <v>20</v>
       </c>
       <c r="B28" s="406" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="C28" s="403" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="D28" s="400">
         <v>54001016498</v>
@@ -28955,10 +29037,10 @@
         <v>21</v>
       </c>
       <c r="B29" s="406" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="C29" s="403" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
       <c r="D29" s="400">
         <v>1024020468</v>
@@ -28982,10 +29064,10 @@
         <v>22</v>
       </c>
       <c r="B30" s="406" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="C30" s="403" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="D30" s="400">
         <v>1027060639</v>
@@ -29009,10 +29091,10 @@
         <v>23</v>
       </c>
       <c r="B31" s="406" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="C31" s="403" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="D31" s="400">
         <v>57001008871</v>
@@ -29036,10 +29118,10 @@
         <v>24</v>
       </c>
       <c r="B32" s="406" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="C32" s="403" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="D32" s="400">
         <v>1019029100</v>
@@ -29063,10 +29145,10 @@
         <v>25</v>
       </c>
       <c r="B33" s="406" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="C33" s="403" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="D33" s="400">
         <v>1032004804</v>
@@ -29090,10 +29172,10 @@
         <v>26</v>
       </c>
       <c r="B34" s="407" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="C34" s="404" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="D34" s="402">
         <v>1001008305</v>
@@ -29117,10 +29199,10 @@
         <v>27</v>
       </c>
       <c r="B35" s="403" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="C35" s="403" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="D35" s="400">
         <v>1003001453</v>
@@ -29144,10 +29226,10 @@
         <v>28</v>
       </c>
       <c r="B36" s="403" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="C36" s="403" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="D36" s="400">
         <v>61003002659</v>
@@ -29171,10 +29253,10 @@
         <v>29</v>
       </c>
       <c r="B37" s="403" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="C37" s="403" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="D37" s="400">
         <v>1019016805</v>
@@ -29198,10 +29280,10 @@
         <v>30</v>
       </c>
       <c r="B38" s="403" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="C38" s="403" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="D38" s="400">
         <v>1001060855</v>
@@ -29225,10 +29307,10 @@
         <v>31</v>
       </c>
       <c r="B39" s="403" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="C39" s="403" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="D39" s="400">
         <v>1021001404</v>
@@ -29252,10 +29334,10 @@
         <v>32</v>
       </c>
       <c r="B40" s="403" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="C40" s="403" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="D40" s="400">
         <v>14001005156</v>
@@ -29279,10 +29361,10 @@
         <v>33</v>
       </c>
       <c r="B41" s="403" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="C41" s="403" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
       <c r="D41" s="400">
         <v>1005041050</v>
@@ -29306,10 +29388,10 @@
         <v>34</v>
       </c>
       <c r="B42" s="403" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
       <c r="C42" s="405" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="D42" s="400">
         <v>1005027236</v>
@@ -29333,10 +29415,10 @@
         <v>35</v>
       </c>
       <c r="B43" s="403" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
       <c r="C43" s="403" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="D43" s="400">
         <v>1031006153</v>
@@ -29360,10 +29442,10 @@
         <v>36</v>
       </c>
       <c r="B44" s="403" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="C44" s="403" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
       <c r="D44" s="400">
         <v>1008054765</v>
@@ -29387,10 +29469,10 @@
         <v>37</v>
       </c>
       <c r="B45" s="403" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="C45" s="403" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="D45" s="400">
         <v>1012001183</v>
@@ -29414,10 +29496,10 @@
         <v>38</v>
       </c>
       <c r="B46" s="403" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="C46" s="403" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
       <c r="D46" s="400">
         <v>1025021607</v>
@@ -29441,10 +29523,10 @@
         <v>39</v>
       </c>
       <c r="B47" s="403" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="C47" s="403" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="D47" s="400">
         <v>1011007155</v>
@@ -29748,7 +29830,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -29794,7 +29876,7 @@
       <c r="E2" s="77"/>
       <c r="F2" s="77"/>
       <c r="G2" s="454" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="H2" s="454"/>
     </row>
@@ -29825,7 +29907,7 @@
       <c r="A5" s="80"/>
       <c r="B5" s="80"/>
       <c r="C5" s="80" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
       <c r="D5" s="80"/>
       <c r="E5" s="80"/>
@@ -31232,7 +31314,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -31281,7 +31363,7 @@
       <c r="E2" s="77"/>
       <c r="F2" s="77"/>
       <c r="G2" s="454" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="H2" s="454"/>
     </row>
@@ -31313,7 +31395,7 @@
       <c r="B5" s="80"/>
       <c r="C5" s="80"/>
       <c r="D5" s="80" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
       <c r="E5" s="80"/>
       <c r="F5" s="80"/>
@@ -31795,11 +31877,11 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L88"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L94"/>
   <sheetViews>
-    <sheetView showGridLines="0" view="pageBreakPreview" topLeftCell="A7" zoomScale="70" zoomScaleSheetLayoutView="70" workbookViewId="0">
-      <selection activeCell="L18" sqref="L18"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A56" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="G76" sqref="G76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -31829,7 +31911,7 @@
       </c>
       <c r="B2" s="115"/>
       <c r="C2" s="454" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="D2" s="455"/>
       <c r="E2" s="155"/>
@@ -31858,7 +31940,7 @@
         <v/>
       </c>
       <c r="B5" s="111" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="C5" s="58"/>
       <c r="D5" s="58"/>
@@ -32210,11 +32292,11 @@
         <v>358</v>
       </c>
       <c r="C36" s="83">
-        <f>SUM(C37:C42)</f>
+        <f>SUM(C37:C41)</f>
         <v>0</v>
       </c>
       <c r="D36" s="83">
-        <f>SUM(D37:D42)</f>
+        <f>SUM(D37:D41)</f>
         <v>0</v>
       </c>
       <c r="E36" s="155"/>
@@ -32268,29 +32350,29 @@
         <v>365</v>
       </c>
       <c r="B41" s="17" t="s">
-        <v>500</v>
+        <v>361</v>
       </c>
       <c r="C41" s="32"/>
       <c r="D41" s="33"/>
       <c r="E41" s="155"/>
     </row>
-    <row r="42" spans="1:5">
-      <c r="A42" s="17" t="s">
-        <v>501</v>
-      </c>
-      <c r="B42" s="17" t="s">
-        <v>361</v>
+    <row r="42" spans="1:5" ht="30">
+      <c r="A42" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="B42" s="16" t="s">
+        <v>28</v>
       </c>
       <c r="C42" s="32"/>
       <c r="D42" s="33"/>
       <c r="E42" s="155"/>
     </row>
-    <row r="43" spans="1:5" ht="30">
+    <row r="43" spans="1:5">
       <c r="A43" s="16" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B43" s="16" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C43" s="32"/>
       <c r="D43" s="33"/>
@@ -32298,10 +32380,10 @@
     </row>
     <row r="44" spans="1:5">
       <c r="A44" s="16" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B44" s="16" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C44" s="32"/>
       <c r="D44" s="33"/>
@@ -32309,10 +32391,10 @@
     </row>
     <row r="45" spans="1:5">
       <c r="A45" s="16" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B45" s="16" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C45" s="32"/>
       <c r="D45" s="33"/>
@@ -32320,38 +32402,38 @@
     </row>
     <row r="46" spans="1:5">
       <c r="A46" s="16" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B46" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="C46" s="32"/>
-      <c r="D46" s="33"/>
+        <v>297</v>
+      </c>
+      <c r="C46" s="83">
+        <f>SUM(C47:C49)</f>
+        <v>0</v>
+      </c>
+      <c r="D46" s="83">
+        <f>SUM(D47:D49)</f>
+        <v>0</v>
+      </c>
       <c r="E46" s="155"/>
     </row>
     <row r="47" spans="1:5">
-      <c r="A47" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="B47" s="16" t="s">
-        <v>297</v>
-      </c>
-      <c r="C47" s="83">
-        <f>SUM(C48:C50)</f>
-        <v>0</v>
-      </c>
-      <c r="D47" s="83">
-        <f>SUM(D48:D50)</f>
-        <v>0</v>
-      </c>
+      <c r="A47" s="97" t="s">
+        <v>371</v>
+      </c>
+      <c r="B47" s="97" t="s">
+        <v>374</v>
+      </c>
+      <c r="C47" s="32"/>
+      <c r="D47" s="33"/>
       <c r="E47" s="155"/>
     </row>
     <row r="48" spans="1:5">
       <c r="A48" s="97" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="B48" s="97" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="C48" s="32"/>
       <c r="D48" s="33"/>
@@ -32359,82 +32441,82 @@
     </row>
     <row r="49" spans="1:5">
       <c r="A49" s="97" t="s">
-        <v>372</v>
+        <v>375</v>
       </c>
       <c r="B49" s="97" t="s">
-        <v>373</v>
+        <v>376</v>
       </c>
       <c r="C49" s="32"/>
       <c r="D49" s="33"/>
       <c r="E49" s="155"/>
     </row>
-    <row r="50" spans="1:5">
-      <c r="A50" s="97" t="s">
-        <v>375</v>
-      </c>
-      <c r="B50" s="97" t="s">
-        <v>376</v>
+    <row r="50" spans="1:5" ht="26.25" customHeight="1">
+      <c r="A50" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="B50" s="16" t="s">
+        <v>29</v>
       </c>
       <c r="C50" s="32"/>
       <c r="D50" s="33"/>
       <c r="E50" s="155"/>
     </row>
-    <row r="51" spans="1:5" ht="26.25" customHeight="1">
+    <row r="51" spans="1:5">
       <c r="A51" s="16" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B51" s="16" t="s">
-        <v>29</v>
+        <v>6</v>
       </c>
       <c r="C51" s="32"/>
       <c r="D51" s="33"/>
       <c r="E51" s="155"/>
     </row>
-    <row r="52" spans="1:5">
-      <c r="A52" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="B52" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="C52" s="32"/>
-      <c r="D52" s="33"/>
+    <row r="52" spans="1:5" ht="30">
+      <c r="A52" s="14">
+        <v>1.3</v>
+      </c>
+      <c r="B52" s="87" t="s">
+        <v>414</v>
+      </c>
+      <c r="C52" s="84">
+        <f>SUM(C53:C54)</f>
+        <v>0</v>
+      </c>
+      <c r="D52" s="84">
+        <f>SUM(D53:D54)</f>
+        <v>0</v>
+      </c>
       <c r="E52" s="155"/>
     </row>
     <row r="53" spans="1:5" ht="30">
-      <c r="A53" s="14">
-        <v>1.3</v>
-      </c>
-      <c r="B53" s="87" t="s">
-        <v>414</v>
-      </c>
-      <c r="C53" s="84">
-        <f>SUM(C54:C55)</f>
-        <v>0</v>
-      </c>
-      <c r="D53" s="84">
-        <f>SUM(D54:D55)</f>
-        <v>0</v>
-      </c>
+      <c r="A53" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="B53" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="C53" s="32"/>
+      <c r="D53" s="33"/>
       <c r="E53" s="155"/>
     </row>
-    <row r="54" spans="1:5" ht="30">
+    <row r="54" spans="1:5">
       <c r="A54" s="16" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B54" s="16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C54" s="32"/>
       <c r="D54" s="33"/>
       <c r="E54" s="155"/>
     </row>
     <row r="55" spans="1:5">
-      <c r="A55" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="B55" s="16" t="s">
-        <v>47</v>
+      <c r="A55" s="14">
+        <v>1.4</v>
+      </c>
+      <c r="B55" s="14" t="s">
+        <v>416</v>
       </c>
       <c r="C55" s="32"/>
       <c r="D55" s="33"/>
@@ -32442,129 +32524,129 @@
     </row>
     <row r="56" spans="1:5">
       <c r="A56" s="14">
-        <v>1.4</v>
+        <v>1.5</v>
       </c>
       <c r="B56" s="14" t="s">
-        <v>416</v>
-      </c>
-      <c r="C56" s="32"/>
-      <c r="D56" s="33"/>
+        <v>7</v>
+      </c>
+      <c r="C56" s="36"/>
+      <c r="D56" s="39"/>
       <c r="E56" s="155"/>
     </row>
     <row r="57" spans="1:5">
       <c r="A57" s="14">
-        <v>1.5</v>
-      </c>
-      <c r="B57" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="C57" s="36"/>
-      <c r="D57" s="39"/>
+        <v>1.6</v>
+      </c>
+      <c r="B57" s="44" t="s">
+        <v>8</v>
+      </c>
+      <c r="C57" s="84">
+        <f>SUM(C58:C62)</f>
+        <v>0</v>
+      </c>
+      <c r="D57" s="84">
+        <f>SUM(D58:D62)</f>
+        <v>0</v>
+      </c>
       <c r="E57" s="155"/>
     </row>
     <row r="58" spans="1:5">
-      <c r="A58" s="14">
-        <v>1.6</v>
-      </c>
-      <c r="B58" s="44" t="s">
-        <v>8</v>
-      </c>
-      <c r="C58" s="84">
-        <f>SUM(C59:C63)</f>
-        <v>0</v>
-      </c>
-      <c r="D58" s="84">
-        <f>SUM(D59:D63)</f>
-        <v>0</v>
-      </c>
+      <c r="A58" s="16" t="s">
+        <v>298</v>
+      </c>
+      <c r="B58" s="45" t="s">
+        <v>52</v>
+      </c>
+      <c r="C58" s="36"/>
+      <c r="D58" s="39"/>
       <c r="E58" s="155"/>
     </row>
-    <row r="59" spans="1:5">
+    <row r="59" spans="1:5" ht="30">
       <c r="A59" s="16" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="B59" s="45" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C59" s="36"/>
       <c r="D59" s="39"/>
       <c r="E59" s="155"/>
     </row>
-    <row r="60" spans="1:5" ht="30">
+    <row r="60" spans="1:5">
       <c r="A60" s="16" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="B60" s="45" t="s">
-        <v>54</v>
-      </c>
-      <c r="C60" s="36"/>
+        <v>53</v>
+      </c>
+      <c r="C60" s="39"/>
       <c r="D60" s="39"/>
       <c r="E60" s="155"/>
     </row>
     <row r="61" spans="1:5">
       <c r="A61" s="16" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="B61" s="45" t="s">
-        <v>53</v>
-      </c>
-      <c r="C61" s="39"/>
+        <v>27</v>
+      </c>
+      <c r="C61" s="36"/>
       <c r="D61" s="39"/>
       <c r="E61" s="155"/>
     </row>
     <row r="62" spans="1:5">
       <c r="A62" s="16" t="s">
-        <v>301</v>
-      </c>
-      <c r="B62" s="45" t="s">
-        <v>27</v>
+        <v>337</v>
+      </c>
+      <c r="B62" s="221" t="s">
+        <v>338</v>
       </c>
       <c r="C62" s="36"/>
-      <c r="D62" s="39"/>
+      <c r="D62" s="222"/>
       <c r="E62" s="155"/>
     </row>
     <row r="63" spans="1:5">
-      <c r="A63" s="16" t="s">
-        <v>337</v>
-      </c>
-      <c r="B63" s="221" t="s">
-        <v>338</v>
-      </c>
-      <c r="C63" s="36"/>
-      <c r="D63" s="222"/>
+      <c r="A63" s="13">
+        <v>2</v>
+      </c>
+      <c r="B63" s="46" t="s">
+        <v>106</v>
+      </c>
+      <c r="C63" s="292"/>
+      <c r="D63" s="119">
+        <f>SUM(D64:D69)</f>
+        <v>0</v>
+      </c>
       <c r="E63" s="155"/>
     </row>
     <row r="64" spans="1:5">
-      <c r="A64" s="13">
-        <v>2</v>
-      </c>
-      <c r="B64" s="46" t="s">
-        <v>106</v>
+      <c r="A64" s="15">
+        <v>2.1</v>
+      </c>
+      <c r="B64" s="47" t="s">
+        <v>100</v>
       </c>
       <c r="C64" s="292"/>
-      <c r="D64" s="119">
-        <f>SUM(D65:D70)</f>
-        <v>0</v>
-      </c>
+      <c r="D64" s="41"/>
       <c r="E64" s="155"/>
     </row>
     <row r="65" spans="1:5">
       <c r="A65" s="15">
-        <v>2.1</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="B65" s="47" t="s">
-        <v>100</v>
-      </c>
-      <c r="C65" s="292"/>
-      <c r="D65" s="41"/>
+        <v>104</v>
+      </c>
+      <c r="C65" s="294"/>
+      <c r="D65" s="42"/>
       <c r="E65" s="155"/>
     </row>
     <row r="66" spans="1:5">
       <c r="A66" s="15">
-        <v>2.2000000000000002</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="B66" s="47" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C66" s="294"/>
       <c r="D66" s="42"/>
@@ -32572,10 +32654,10 @@
     </row>
     <row r="67" spans="1:5">
       <c r="A67" s="15">
-        <v>2.2999999999999998</v>
+        <v>2.4</v>
       </c>
       <c r="B67" s="47" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="C67" s="294"/>
       <c r="D67" s="42"/>
@@ -32583,10 +32665,10 @@
     </row>
     <row r="68" spans="1:5">
       <c r="A68" s="15">
-        <v>2.4</v>
+        <v>2.5</v>
       </c>
       <c r="B68" s="47" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C68" s="294"/>
       <c r="D68" s="42"/>
@@ -32594,179 +32676,249 @@
     </row>
     <row r="69" spans="1:5">
       <c r="A69" s="15">
-        <v>2.5</v>
+        <v>2.6</v>
       </c>
       <c r="B69" s="47" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C69" s="294"/>
       <c r="D69" s="42"/>
       <c r="E69" s="155"/>
     </row>
-    <row r="70" spans="1:5">
-      <c r="A70" s="15">
-        <v>2.6</v>
-      </c>
-      <c r="B70" s="47" t="s">
-        <v>102</v>
-      </c>
-      <c r="C70" s="294"/>
-      <c r="D70" s="42"/>
-      <c r="E70" s="155"/>
+    <row r="70" spans="1:5" s="2" customFormat="1">
+      <c r="A70" s="13">
+        <v>3</v>
+      </c>
+      <c r="B70" s="290" t="s">
+        <v>449</v>
+      </c>
+      <c r="C70" s="293"/>
+      <c r="D70" s="291"/>
+      <c r="E70" s="105"/>
     </row>
     <row r="71" spans="1:5" s="2" customFormat="1">
       <c r="A71" s="13">
-        <v>3</v>
-      </c>
-      <c r="B71" s="290" t="s">
-        <v>449</v>
-      </c>
-      <c r="C71" s="293"/>
-      <c r="D71" s="291"/>
+        <v>4</v>
+      </c>
+      <c r="B71" s="13" t="s">
+        <v>252</v>
+      </c>
+      <c r="C71" s="293">
+        <f>SUM(C72:C73)</f>
+        <v>0</v>
+      </c>
+      <c r="D71" s="85">
+        <f>SUM(D72:D73)</f>
+        <v>0</v>
+      </c>
       <c r="E71" s="105"/>
     </row>
     <row r="72" spans="1:5" s="2" customFormat="1">
-      <c r="A72" s="13">
-        <v>4</v>
-      </c>
-      <c r="B72" s="13" t="s">
-        <v>252</v>
-      </c>
-      <c r="C72" s="293">
-        <f>SUM(C73:C74)</f>
-        <v>0</v>
-      </c>
-      <c r="D72" s="85">
-        <f>SUM(D73:D74)</f>
-        <v>0</v>
-      </c>
+      <c r="A72" s="15">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="B72" s="15" t="s">
+        <v>253</v>
+      </c>
+      <c r="C72" s="8"/>
+      <c r="D72" s="8"/>
       <c r="E72" s="105"/>
     </row>
     <row r="73" spans="1:5" s="2" customFormat="1">
       <c r="A73" s="15">
-        <v>4.0999999999999996</v>
+        <v>4.2</v>
       </c>
       <c r="B73" s="15" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="C73" s="8"/>
       <c r="D73" s="8"/>
       <c r="E73" s="105"/>
     </row>
-    <row r="74" spans="1:5" s="2" customFormat="1">
-      <c r="A74" s="15">
-        <v>4.2</v>
-      </c>
-      <c r="B74" s="15" t="s">
-        <v>254</v>
+    <row r="74" spans="1:5" s="2" customFormat="1" ht="15.75" thickBot="1">
+      <c r="A74" s="13">
+        <v>5</v>
+      </c>
+      <c r="B74" s="288" t="s">
+        <v>280</v>
       </c>
       <c r="C74" s="8"/>
-      <c r="D74" s="8"/>
+      <c r="D74" s="85"/>
       <c r="E74" s="105"/>
     </row>
-    <row r="75" spans="1:5" s="2" customFormat="1">
-      <c r="A75" s="13">
-        <v>5</v>
-      </c>
-      <c r="B75" s="288" t="s">
-        <v>280</v>
-      </c>
-      <c r="C75" s="8"/>
-      <c r="D75" s="85"/>
+    <row r="75" spans="1:5" s="2" customFormat="1" ht="26.25" thickBot="1">
+      <c r="A75" s="474">
+        <v>6</v>
+      </c>
+      <c r="B75" s="475" t="s">
+        <v>614</v>
+      </c>
+      <c r="C75" s="12">
+        <v>0</v>
+      </c>
+      <c r="D75" s="473">
+        <v>0</v>
+      </c>
       <c r="E75" s="105"/>
     </row>
-    <row r="76" spans="1:5" s="2" customFormat="1">
-      <c r="A76" s="398"/>
-      <c r="B76" s="398"/>
+    <row r="76" spans="1:5" s="2" customFormat="1" ht="15.75" thickBot="1">
+      <c r="A76" s="476">
+        <v>6.1</v>
+      </c>
+      <c r="B76" s="477" t="s">
+        <v>68</v>
+      </c>
       <c r="C76" s="12"/>
-      <c r="D76" s="12"/>
+      <c r="D76" s="473"/>
       <c r="E76" s="105"/>
     </row>
-    <row r="77" spans="1:5" s="2" customFormat="1">
-      <c r="A77" s="459" t="s">
+    <row r="77" spans="1:5" s="2" customFormat="1" ht="15.75" thickBot="1">
+      <c r="A77" s="476">
+        <v>6.2</v>
+      </c>
+      <c r="B77" s="477" t="s">
+        <v>74</v>
+      </c>
+      <c r="C77" s="12"/>
+      <c r="D77" s="473"/>
+      <c r="E77" s="105"/>
+    </row>
+    <row r="78" spans="1:5" s="2" customFormat="1" ht="15.75" thickBot="1">
+      <c r="A78" s="476">
+        <v>6.3</v>
+      </c>
+      <c r="B78" s="477" t="s">
+        <v>69</v>
+      </c>
+      <c r="C78" s="12"/>
+      <c r="D78" s="473"/>
+      <c r="E78" s="105"/>
+    </row>
+    <row r="79" spans="1:5" s="2" customFormat="1" ht="15.75" thickBot="1">
+      <c r="A79" s="476">
+        <v>6.4</v>
+      </c>
+      <c r="B79" s="477" t="s">
+        <v>615</v>
+      </c>
+      <c r="C79" s="12"/>
+      <c r="D79" s="473"/>
+      <c r="E79" s="105"/>
+    </row>
+    <row r="80" spans="1:5" s="2" customFormat="1" ht="15.75" thickBot="1">
+      <c r="A80" s="476">
+        <v>6.5</v>
+      </c>
+      <c r="B80" s="477" t="s">
+        <v>78</v>
+      </c>
+      <c r="C80" s="12"/>
+      <c r="D80" s="473"/>
+      <c r="E80" s="105"/>
+    </row>
+    <row r="81" spans="1:9" s="2" customFormat="1" ht="15.75" thickBot="1">
+      <c r="A81" s="476">
+        <v>6.6</v>
+      </c>
+      <c r="B81" s="477" t="s">
+        <v>8</v>
+      </c>
+      <c r="C81" s="12"/>
+      <c r="D81" s="473"/>
+      <c r="E81" s="105"/>
+    </row>
+    <row r="82" spans="1:9" s="2" customFormat="1">
+      <c r="A82" s="398"/>
+      <c r="B82" s="398"/>
+      <c r="C82" s="12"/>
+      <c r="D82" s="12"/>
+      <c r="E82" s="105"/>
+    </row>
+    <row r="83" spans="1:9" s="2" customFormat="1">
+      <c r="A83" s="459" t="s">
+        <v>500</v>
+      </c>
+      <c r="B83" s="459"/>
+      <c r="C83" s="459"/>
+      <c r="D83" s="459"/>
+      <c r="E83" s="105"/>
+    </row>
+    <row r="84" spans="1:9" s="2" customFormat="1">
+      <c r="A84" s="398"/>
+      <c r="B84" s="398"/>
+      <c r="C84" s="12"/>
+      <c r="D84" s="12"/>
+      <c r="E84" s="105"/>
+    </row>
+    <row r="85" spans="1:9" s="22" customFormat="1" ht="12.75"/>
+    <row r="86" spans="1:9" s="2" customFormat="1">
+      <c r="A86" s="69" t="s">
+        <v>107</v>
+      </c>
+      <c r="E86" s="5"/>
+    </row>
+    <row r="87" spans="1:9" s="2" customFormat="1">
+      <c r="E87"/>
+      <c r="F87"/>
+      <c r="G87"/>
+      <c r="H87"/>
+      <c r="I87"/>
+    </row>
+    <row r="88" spans="1:9" s="2" customFormat="1">
+      <c r="D88" s="12"/>
+      <c r="E88"/>
+      <c r="F88"/>
+      <c r="G88"/>
+      <c r="H88"/>
+      <c r="I88"/>
+    </row>
+    <row r="89" spans="1:9" s="2" customFormat="1">
+      <c r="A89"/>
+      <c r="B89" s="43" t="s">
+        <v>501</v>
+      </c>
+      <c r="D89" s="12"/>
+      <c r="E89"/>
+      <c r="F89"/>
+      <c r="G89"/>
+      <c r="H89"/>
+      <c r="I89"/>
+    </row>
+    <row r="90" spans="1:9" s="2" customFormat="1">
+      <c r="A90"/>
+      <c r="B90" s="460" t="s">
         <v>502</v>
       </c>
-      <c r="B77" s="459"/>
-      <c r="C77" s="459"/>
-      <c r="D77" s="459"/>
-      <c r="E77" s="105"/>
-    </row>
-    <row r="78" spans="1:5" s="2" customFormat="1">
-      <c r="A78" s="398"/>
-      <c r="B78" s="398"/>
-      <c r="C78" s="12"/>
-      <c r="D78" s="12"/>
-      <c r="E78" s="105"/>
-    </row>
-    <row r="79" spans="1:5" s="22" customFormat="1" ht="12.75"/>
-    <row r="80" spans="1:5" s="2" customFormat="1">
-      <c r="A80" s="69" t="s">
-        <v>107</v>
-      </c>
-      <c r="E80" s="5"/>
-    </row>
-    <row r="81" spans="1:9" s="2" customFormat="1">
-      <c r="E81"/>
-      <c r="F81"/>
-      <c r="G81"/>
-      <c r="H81"/>
-      <c r="I81"/>
-    </row>
-    <row r="82" spans="1:9" s="2" customFormat="1">
-      <c r="D82" s="12"/>
-      <c r="E82"/>
-      <c r="F82"/>
-      <c r="G82"/>
-      <c r="H82"/>
-      <c r="I82"/>
-    </row>
-    <row r="83" spans="1:9" s="2" customFormat="1">
-      <c r="A83"/>
-      <c r="B83" s="43" t="s">
+      <c r="C90" s="460"/>
+      <c r="D90" s="460"/>
+      <c r="E90"/>
+      <c r="F90"/>
+      <c r="G90"/>
+      <c r="H90"/>
+      <c r="I90"/>
+    </row>
+    <row r="91" spans="1:9" customFormat="1" ht="12.75">
+      <c r="B91" s="65" t="s">
         <v>503</v>
       </c>
-      <c r="D83" s="12"/>
-      <c r="E83"/>
-      <c r="F83"/>
-      <c r="G83"/>
-      <c r="H83"/>
-      <c r="I83"/>
-    </row>
-    <row r="84" spans="1:9" s="2" customFormat="1">
-      <c r="A84"/>
-      <c r="B84" s="460" t="s">
+    </row>
+    <row r="92" spans="1:9" s="2" customFormat="1">
+      <c r="A92" s="11"/>
+      <c r="B92" s="460" t="s">
         <v>504</v>
       </c>
-      <c r="C84" s="460"/>
-      <c r="D84" s="460"/>
-      <c r="E84"/>
-      <c r="F84"/>
-      <c r="G84"/>
-      <c r="H84"/>
-      <c r="I84"/>
-    </row>
-    <row r="85" spans="1:9" customFormat="1" ht="12.75">
-      <c r="B85" s="65" t="s">
-        <v>505</v>
-      </c>
-    </row>
-    <row r="86" spans="1:9" s="2" customFormat="1">
-      <c r="A86" s="11"/>
-      <c r="B86" s="460" t="s">
-        <v>506</v>
-      </c>
-      <c r="C86" s="460"/>
-      <c r="D86" s="460"/>
-    </row>
-    <row r="87" spans="1:9" s="22" customFormat="1" ht="12.75"/>
-    <row r="88" spans="1:9" s="22" customFormat="1" ht="12.75"/>
+      <c r="C92" s="460"/>
+      <c r="D92" s="460"/>
+    </row>
+    <row r="93" spans="1:9" s="22" customFormat="1" ht="12.75"/>
+    <row r="94" spans="1:9" s="22" customFormat="1" ht="12.75"/>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="C2:D2"/>
-    <mergeCell ref="A77:D77"/>
-    <mergeCell ref="B84:D84"/>
-    <mergeCell ref="B86:D86"/>
+    <mergeCell ref="A83:D83"/>
+    <mergeCell ref="B90:D90"/>
+    <mergeCell ref="B92:D92"/>
   </mergeCells>
   <printOptions gridLines="1"/>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>